<commit_message>
Updated Traceability Link Matrices with all classes.
</commit_message>
<xml_diff>
--- a/documentation/traceability_link_matrices/Client Traceability Link Matrix.xlsx
+++ b/documentation/traceability_link_matrices/Client Traceability Link Matrix.xlsx
@@ -11,17 +11,89 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="47">
   <si>
     <t>Client Traceability Link Matrix</t>
   </si>
   <si>
+    <t>AccountHandler</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>GameBoardController</t>
+  </si>
+  <si>
+    <t>HomeController</t>
+  </si>
+  <si>
+    <t>LoginController</t>
+  </si>
+  <si>
+    <t>RegisterController</t>
+  </si>
+  <si>
+    <t>BoardSquare</t>
+  </si>
+  <si>
+    <t>CatPiece</t>
+  </si>
+  <si>
+    <t>DenSquare</t>
+  </si>
+  <si>
+    <t>DogPiece</t>
+  </si>
+  <si>
+    <t>ElephantPiece</t>
+  </si>
+  <si>
+    <t>FoxPiece</t>
+  </si>
+  <si>
+    <t>GameBoard</t>
+  </si>
+  <si>
+    <t>JungleGame</t>
+  </si>
+  <si>
+    <t>JungleGamePiece</t>
+  </si>
+  <si>
+    <t>LeopardPiece</t>
+  </si>
+  <si>
+    <t>LionPiece</t>
+  </si>
+  <si>
+    <t>RatPiece</t>
+  </si>
+  <si>
+    <t>RiverSquare</t>
+  </si>
+  <si>
+    <t>TigerPiece</t>
+  </si>
+  <si>
+    <t>TrapSquare</t>
+  </si>
+  <si>
+    <t>AuthTokenManager</t>
+  </si>
+  <si>
+    <t>GamesManager</t>
+  </si>
+  <si>
+    <t>InviteManager</t>
+  </si>
+  <si>
+    <t>JungleClient</t>
+  </si>
+  <si>
     <t>NetworkListener</t>
   </si>
   <si>
-    <t>JungleClient</t>
-  </si>
-  <si>
     <t>CreateGameHandler</t>
   </si>
   <si>
@@ -43,40 +115,7 @@
     <t>RegistrationHandler</t>
   </si>
   <si>
-    <t>AccountHandler</t>
-  </si>
-  <si>
-    <t>RegisterController</t>
-  </si>
-  <si>
-    <t>LoginController</t>
-  </si>
-  <si>
-    <t>GameBoardController</t>
-  </si>
-  <si>
-    <t>HomeController</t>
-  </si>
-  <si>
-    <t>AuthTokenManager</t>
-  </si>
-  <si>
-    <t>GamesManager</t>
-  </si>
-  <si>
-    <t>Invite Manager</t>
-  </si>
-  <si>
-    <t>Jungle Game</t>
-  </si>
-  <si>
-    <t>GameBoard</t>
-  </si>
-  <si>
-    <t>GamePiece</t>
-  </si>
-  <si>
-    <t>Board quare</t>
+    <t>InviteListCell</t>
   </si>
   <si>
     <t>#1: Register to the system</t>
@@ -95,9 +134,6 @@
   </si>
   <si>
     <t>#5: Quit Game</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>#6: Unregister from System</t>
@@ -261,10 +297,10 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -293,21 +329,39 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="45.43"/>
     <col customWidth="1" min="2" max="2" width="23.14"/>
-    <col customWidth="1" min="3" max="3" width="21.57"/>
-    <col customWidth="1" min="4" max="4" width="26.71"/>
+    <col customWidth="1" min="3" max="3" width="14.43"/>
+    <col customWidth="1" min="4" max="4" width="30.57"/>
     <col customWidth="1" min="5" max="5" width="23.14"/>
-    <col customWidth="1" min="6" max="6" width="27.14"/>
-    <col customWidth="1" min="7" max="7" width="27.86"/>
-    <col customWidth="1" min="8" max="9" width="21.57"/>
-    <col customWidth="1" min="10" max="10" width="28.29"/>
-    <col customWidth="1" min="11" max="11" width="21.57"/>
-    <col customWidth="1" min="12" max="12" width="26.57"/>
-    <col customWidth="1" min="13" max="13" width="22.14"/>
-    <col customWidth="1" min="14" max="14" width="28.29"/>
-    <col customWidth="1" min="15" max="15" width="21.57"/>
+    <col customWidth="1" min="6" max="6" width="24.29"/>
+    <col customWidth="1" min="7" max="7" width="27.29"/>
+    <col customWidth="1" min="8" max="8" width="21.57"/>
+    <col customWidth="1" min="9" max="9" width="15.86"/>
+    <col customWidth="1" min="10" max="10" width="20.14"/>
+    <col customWidth="1" min="11" max="11" width="16.43"/>
+    <col customWidth="1" min="12" max="12" width="19.86"/>
+    <col customWidth="1" min="13" max="13" width="16.86"/>
+    <col customWidth="1" min="14" max="14" width="20.43"/>
+    <col customWidth="1" min="15" max="15" width="19.14"/>
     <col customWidth="1" min="16" max="16" width="25.57"/>
-    <col customWidth="1" min="17" max="17" width="21.57"/>
-    <col customWidth="1" min="18" max="22" width="19.29"/>
+    <col customWidth="1" min="17" max="17" width="19.14"/>
+    <col customWidth="1" min="18" max="18" width="17.14"/>
+    <col customWidth="1" min="19" max="19" width="14.57"/>
+    <col customWidth="1" min="20" max="20" width="19.29"/>
+    <col customWidth="1" min="21" max="21" width="17.43"/>
+    <col customWidth="1" min="22" max="22" width="18.0"/>
+    <col customWidth="1" min="23" max="23" width="26.0"/>
+    <col customWidth="1" min="24" max="24" width="23.71"/>
+    <col customWidth="1" min="25" max="25" width="20.14"/>
+    <col customWidth="1" min="26" max="26" width="18.71"/>
+    <col customWidth="1" min="27" max="27" width="23.29"/>
+    <col customWidth="1" min="28" max="28" width="28.71"/>
+    <col customWidth="1" min="29" max="29" width="23.0"/>
+    <col customWidth="1" min="30" max="30" width="27.14"/>
+    <col customWidth="1" min="31" max="31" width="25.43"/>
+    <col customWidth="1" min="32" max="32" width="20.14"/>
+    <col customWidth="1" min="33" max="33" width="20.43"/>
+    <col customWidth="1" min="34" max="34" width="27.86"/>
+    <col customWidth="1" min="35" max="35" width="20.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="40.5" customHeight="1">
@@ -334,9 +388,22 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
-      <c r="V1" s="3"/>
-    </row>
-    <row r="2" ht="36.75" customHeight="1">
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="3"/>
+    </row>
+    <row r="2" ht="36.0" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -401,436 +468,690 @@
       <c r="V2" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" ht="36.75" customHeight="1">
+      <c r="W2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="G3" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="9"/>
       <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="10"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="9"/>
       <c r="V3" s="11"/>
-    </row>
-    <row r="4" ht="36.75" customHeight="1">
+      <c r="W3" s="11"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" s="11"/>
+    </row>
+    <row r="4">
       <c r="A4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="U4" s="10"/>
-      <c r="V4" s="11"/>
-    </row>
-    <row r="5" ht="36.75" customHeight="1">
+      <c r="G4" s="10"/>
+      <c r="H4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="11"/>
+    </row>
+    <row r="5">
       <c r="A5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
       <c r="V5" s="11"/>
-    </row>
-    <row r="6" ht="36.75" customHeight="1">
+      <c r="W5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="11"/>
+    </row>
+    <row r="6">
       <c r="A6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="G6" s="10"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S6" s="10"/>
-      <c r="T6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="U6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="9"/>
       <c r="V6" s="13"/>
-    </row>
-    <row r="7" ht="36.75" customHeight="1">
+      <c r="W6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="T7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="U7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="9"/>
       <c r="V7" s="13"/>
-    </row>
-    <row r="8" ht="36.75" customHeight="1">
+      <c r="W7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="13"/>
+    </row>
+    <row r="8">
       <c r="A8" s="7" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
       <c r="V8" s="11"/>
-    </row>
-    <row r="9" ht="36.75" customHeight="1">
+      <c r="W8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI8" s="11"/>
+    </row>
+    <row r="9">
       <c r="A9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
       <c r="V9" s="13"/>
-    </row>
-    <row r="10" ht="36.75" customHeight="1">
+      <c r="W9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="13"/>
+    </row>
+    <row r="10">
       <c r="A10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
       <c r="V10" s="11"/>
-    </row>
-    <row r="11" ht="36.75" customHeight="1">
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI10" s="11"/>
+    </row>
+    <row r="11">
       <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
       <c r="V11" s="11"/>
-    </row>
-    <row r="12" ht="36.75" customHeight="1">
+      <c r="W11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+    </row>
+    <row r="12">
       <c r="A12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="10"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="T12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="U12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="V12" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" ht="36.75" customHeight="1">
+      <c r="G12" s="10"/>
+      <c r="H12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="10"/>
+    </row>
+    <row r="13">
       <c r="A13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="T13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="U13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="9"/>
       <c r="V13" s="13"/>
+      <c r="W13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="13"/>
+      <c r="AI13" s="13"/>
     </row>
     <row r="14">
       <c r="A14" s="14"/>
@@ -3754,48 +4075,9 @@
     <row r="987">
       <c r="A987" s="14"/>
     </row>
-    <row r="988">
-      <c r="A988" s="14"/>
-    </row>
-    <row r="989">
-      <c r="A989" s="14"/>
-    </row>
-    <row r="990">
-      <c r="A990" s="14"/>
-    </row>
-    <row r="991">
-      <c r="A991" s="14"/>
-    </row>
-    <row r="992">
-      <c r="A992" s="14"/>
-    </row>
-    <row r="993">
-      <c r="A993" s="14"/>
-    </row>
-    <row r="994">
-      <c r="A994" s="14"/>
-    </row>
-    <row r="995">
-      <c r="A995" s="14"/>
-    </row>
-    <row r="996">
-      <c r="A996" s="14"/>
-    </row>
-    <row r="997">
-      <c r="A997" s="14"/>
-    </row>
-    <row r="998">
-      <c r="A998" s="14"/>
-    </row>
-    <row r="999">
-      <c r="A999" s="14"/>
-    </row>
-    <row r="1000">
-      <c r="A1000" s="14"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A1:AI1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" location="heading=h.s7t9mh5d6b9p" ref="A3"/>

</xml_diff>